<commit_message>
new data day 08/09/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url.xlsx
+++ b/Data/Draft/url.xlsx
@@ -27,198 +27,216 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899459708882708?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899367455558600?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899272168901462?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899200088908670?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899184368910242?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899123735582972?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899061125589233?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899054682256544?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899016092260403?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/899000572261955?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898961368932542?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898923745602971?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898913878937291?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898900665605279?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898862848942394?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898599368968742?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898808495614496?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898564672305545?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898482272313785?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898474662314546?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898472682314744?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898453172316695?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898430045652341?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898387572323255?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898370662324946?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898365232325489?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898337255661620?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898325312329481?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898201115675234?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898210292340983?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/898148449013834?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897942109034468?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897835842378428?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897774829051196?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897781715717174?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897753055720040?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897736879054991?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897662795729066?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897539849074694?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897225289106150?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897165679112111?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/897074259121253?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896991495796196?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896947705800575?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896941309134548?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896883839140295?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896530139175665?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896509692511043?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896523515842994?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896463639182315?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896452339183445?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/896234275871918?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/895902845905061?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/895967109231968?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/895566025938743?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/895539295941416?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/895000689328610?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/894880162673996?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/894861879342491?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/894669119361767?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/894629792699033?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/894487949379884?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/894376336057712?ref=embed_post</t>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919258186902860?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919233066905372?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://facebook.com/congdongvnexpress/posts/919162696912409?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919171090244903?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919145590247453?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919132723582073?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919123920249620?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919029106925768?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/919017566926922?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918980760263936?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918962380265774?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918751923620153?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918744706954208?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918689860293026?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918654803629865?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918605396968139?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918581103637235?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918489660313046?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918447133650632?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918431176985561?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918423576986321?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918413453654000?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918376946990984?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918360666992612?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918339873661358?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918087240353288?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/918038157024863?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917964633698882?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917896793705666?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917874467041232?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917832740378738?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917650547063624?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917640660397946?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917388803756465?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917257963769549?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917114293783916?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917084130453599?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/917015493793796?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916996130462399?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916982177130461?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916855120476500?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916834553811890?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916441537184525?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916385203856825?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/916339283861417?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/915847620577250?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/915728963922449?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/915627500599262?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/915438470618165?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/915481940613818?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/915163660645646?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/914913977337281?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/914858724009473?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/914697050692307?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/955003353331112?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954956693335778?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954922143339233?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954760723355375?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954530860045028?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954864530011661?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/953983910099723?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954071693424278?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954346793396768?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954868566677924?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/954040196760761?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/953949683436479?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/953685933462854?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/953503266814454?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/953494553481992?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1392,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1467,242 +1485,282 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:1">
+      <c r="A66" s="1" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data and report day 10/09/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url.xlsx
+++ b/Data/Draft/url.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10668" windowHeight="9000"/>
+    <workbookView windowWidth="12455" windowHeight="7367"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
   <si>
     <t>link</t>
   </si>
@@ -237,6 +237,225 @@
   </si>
   <si>
     <t>https://www.facebook.com/thongtinchinhphu/posts/953494553481992?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1086255269533527?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1086230649535989?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1086122076213513?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1086114386214282?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085794356246285?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085761109582943?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085682116257509?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085661669592887?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085642392928148?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085571226268598?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085551786270542?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085543339604720?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085425249616529?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085330646292656?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085144379644616?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1084976309661423?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1085035326322188?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1084972492995138?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1084906223001765?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1083506763141711?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1082872929871761?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1081274030031651?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1081100873382300?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daiphatthanh.sound/posts/1080976443394743?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/848822557336610?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/849594060592793?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/849702150581984?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/848757200676479?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/848031870749012?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847699137448952?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847696394115893?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847467867472079?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847466417472224?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847349824150550?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847349377483928?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/847334830818716?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846978224187710?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846527814232751?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846526880899511?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846520450900154?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845969754288557?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845967747622091?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846246750927524?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845970094288523?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846247574260775?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/846249850927214?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845968380955361?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845848920967307?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845383654347167?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845176004367932?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/845076601044539?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844602777758588?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844747494410783?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844601501092049?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844450401107159?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844178344467698?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844448921107307?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/844025744482958?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/843749261177273?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/843421704543362?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/843416684543864?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/843227264562806?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/842065341345665?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/842028544682678?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/841698508049015?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/841235981428601?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/841096431442556?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/841095008109365?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/840997844785748?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/840995361452663?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/840994084786124?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/840251141527085?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/840251611527038?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -1392,15 +1611,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A72"/>
+  <dimension ref="A1:A146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="4" width="8.88888888888889" style="1"/>
+    <col min="5" max="5" width="17.2222222222222" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
@@ -1763,6 +1984,376 @@
         <v>69</v>
       </c>
     </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
update model and report day 19/09/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url.xlsx
+++ b/Data/Draft/url.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12455" windowHeight="7367"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1613,15 +1613,15 @@
   <sheetPr/>
   <dimension ref="A1:A146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="8.88888888888889" style="1"/>
-    <col min="5" max="5" width="17.2222222222222" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="4" width="8.88571428571429" style="1"/>
+    <col min="5" max="5" width="17.2190476190476" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88571428571429" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
@@ -2355,6 +2355,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" display="https://www.facebook.com/congdongvnexpress/posts/919145590247453?ref=embed_post"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
update crawl code day 29/09/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url.xlsx
+++ b/Data/Draft/url.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="140">
   <si>
     <t>link</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/919258186902860?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/919233066905372?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://facebook.com/congdongvnexpress/posts/919162696912409?ref=embed_post</t>
   </si>
   <si>
     <t>https://www.facebook.com/congdongvnexpress/posts/919171090244903?ref=embed_post</t>
@@ -1611,17 +1602,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A146"/>
+  <dimension ref="A1:A143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" width="8.88571428571429" style="1"/>
-    <col min="5" max="5" width="17.2190476190476" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88571428571429" style="1"/>
+    <col min="1" max="4" width="8.88888888888889" style="1"/>
+    <col min="5" max="5" width="17.2222222222222" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
@@ -1635,7 +1626,7 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1650,7 +1641,7 @@
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1691,17 +1682,17 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -1710,7 +1701,7 @@
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1725,7 +1716,7 @@
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1796,17 +1787,17 @@
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1">
@@ -1925,7 +1916,7 @@
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1940,7 +1931,7 @@
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2291,17 +2282,17 @@
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="1:1">
@@ -2339,24 +2330,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
-      <c r="A144" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1">
-      <c r="A145" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://www.facebook.com/congdongvnexpress/posts/919145590247453?ref=embed_post"/>
+    <hyperlink ref="A3" r:id="rId1" display="https://www.facebook.com/congdongvnexpress/posts/919145590247453?ref=embed_post"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
update data day 06/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url.xlsx
+++ b/Data/Draft/url.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,189 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>link</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553740453703786?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553729650371533?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553678540376644?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553582177052947?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553550293722802?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553496167061548?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553485820395916?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553444653733366?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553062507104914?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vietnamnet.vn/posts/553037987107366?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975771387911742?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975862991235915?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975736464581901?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975655574589990?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975463704609177?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975605017928379?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975440204611527?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975386174616930?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975349314620616?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/975242117964669?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974681104687437?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974644314691116?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974529888035892?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974522554703292?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974472921374922?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974460281376186?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974028761419338?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/974054468083434?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973978714757676?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973868414768706?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973740998114781?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973247471497467?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973216881500526?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973116644843883?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973087828180098?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/973061861516028?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972924911529723?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972903518198529?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972842828204598?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972531128235768?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972480714907476?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972405501581664?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972345411587673?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972303394925208?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972176678271213?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971982841623930?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971551385000409?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/972119654943582?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971528798336001?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971520891670125?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971497368339144?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971467011675513?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971408848347996?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971400278348853?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971330895022458?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/971306731691541?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/970767205078827?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/970713558417525?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/970611185094429?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/970473191774895?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -233,15 +53,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -695,12 +515,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -825,12 +645,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1364,17 +1191,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A62"/>
+  <dimension ref="A1:A213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A213" sqref="$A2:$XFD213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="8.88888888888889" style="1"/>
-    <col min="5" max="5" width="17.2222222222222" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="4" width="8.88571428571429" style="1"/>
+    <col min="5" max="5" width="17.2190476190476" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88571428571429" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
@@ -1382,311 +1209,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A26" s="2"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
+    <row r="154" customFormat="1" spans="1:1">
+      <c r="A154" s="4"/>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
+    <row r="155" customFormat="1"/>
+    <row r="156" customFormat="1"/>
+    <row r="157" customFormat="1"/>
+    <row r="158" customFormat="1"/>
+    <row r="159" customFormat="1" spans="1:1">
+      <c r="A159" s="4"/>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
-      </c>
+    <row r="160" customFormat="1"/>
+    <row r="161" customFormat="1"/>
+    <row r="162" customFormat="1"/>
+    <row r="163" customFormat="1"/>
+    <row r="164" customFormat="1"/>
+    <row r="165" customFormat="1"/>
+    <row r="166" customFormat="1"/>
+    <row r="167" customFormat="1"/>
+    <row r="168" customFormat="1"/>
+    <row r="169" customFormat="1"/>
+    <row r="170" customFormat="1" spans="1:1">
+      <c r="A170" s="5"/>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
+    <row r="171" customFormat="1"/>
+    <row r="172" customFormat="1"/>
+    <row r="173" customFormat="1"/>
+    <row r="174" customFormat="1"/>
+    <row r="175" customFormat="1"/>
+    <row r="176" customFormat="1"/>
+    <row r="177" customFormat="1"/>
+    <row r="178" customFormat="1"/>
+    <row r="179" customFormat="1"/>
+    <row r="180" customFormat="1"/>
+    <row r="181" customFormat="1"/>
+    <row r="182" customFormat="1"/>
+    <row r="183" customFormat="1"/>
+    <row r="184" customFormat="1" spans="1:1">
+      <c r="A184" s="4"/>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
+    <row r="185" customFormat="1"/>
+    <row r="186" customFormat="1"/>
+    <row r="187" customFormat="1"/>
+    <row r="188" customFormat="1"/>
+    <row r="189" customFormat="1"/>
+    <row r="190" customFormat="1"/>
+    <row r="191" customFormat="1"/>
+    <row r="192" customFormat="1"/>
+    <row r="193" customFormat="1"/>
+    <row r="194" customFormat="1"/>
+    <row r="195" customFormat="1"/>
+    <row r="196" customFormat="1"/>
+    <row r="197" customFormat="1"/>
+    <row r="198" customFormat="1"/>
+    <row r="199" customFormat="1"/>
+    <row r="200" customFormat="1"/>
+    <row r="201" customFormat="1"/>
+    <row r="202" customFormat="1"/>
+    <row r="203" customFormat="1"/>
+    <row r="204" customFormat="1"/>
+    <row r="205" customFormat="1"/>
+    <row r="206" customFormat="1"/>
+    <row r="207" customFormat="1"/>
+    <row r="208" customFormat="1" spans="1:1">
+      <c r="A208" s="4"/>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
+    <row r="209" customFormat="1"/>
+    <row r="210" customFormat="1"/>
+    <row r="211" customFormat="1"/>
+    <row r="212" customFormat="1"/>
+    <row r="213" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>